<commit_message>
Laatste foutjes op basis van commentaar Toolkit team
</commit_message>
<xml_diff>
--- a/A00 Documentatie/Toolkit catalogus 20210520.xlsx
+++ b/A00 Documentatie/Toolkit catalogus 20210520.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Botterhuis\Werk\Pr\4440_10\def\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benitm\GIT\HB-Datatoolkit\A00 Documentatie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CB129E8-4478-4E0F-ADC4-322A051E326D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9D46886-B28D-4E0B-80D5-44815F7D79B6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3158DF1D-2F05-4AFC-98CF-1D03CBBCD17C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{3158DF1D-2F05-4AFC-98CF-1D03CBBCD17C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overzicht scripts" sheetId="2" r:id="rId1"/>
@@ -398,9 +398,6 @@
     <t>\S05_Bouw_databases_Benedenrivieren</t>
   </si>
   <si>
-    <t>\S05_Fetchbottom</t>
-  </si>
-  <si>
     <t>\S03_SWAN_WAQUA_Oosterschelde\SCRIPTS\ProcChecks</t>
   </si>
   <si>
@@ -414,6 +411,9 @@
   </si>
   <si>
     <t>\S11_Controle databases WBI2017</t>
+  </si>
+  <si>
+    <t>\S04_Fetchbottom</t>
   </si>
 </sst>
 </file>
@@ -483,7 +483,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -500,11 +500,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -559,6 +570,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1496,21 +1516,21 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B47" sqref="B47"/>
+      <selection pane="bottomRight" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="61.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="61.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.21875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="50.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.28515625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="50.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.6640625" style="1" customWidth="1"/>
-    <col min="6" max="7" width="42.21875" style="3" customWidth="1"/>
-    <col min="8" max="16384" width="61.33203125" style="1"/>
+    <col min="5" max="5" width="20.7109375" style="1" customWidth="1"/>
+    <col min="6" max="7" width="42.28515625" style="3" customWidth="1"/>
+    <col min="8" max="16384" width="61.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="16" customFormat="1" ht="36" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="16" customFormat="1" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>3</v>
       </c>
@@ -1533,12 +1553,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="11" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" s="11" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C2" s="13" t="s">
         <v>18</v>
@@ -1554,7 +1574,7 @@
       </c>
       <c r="G2" s="10"/>
     </row>
-    <row r="3" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -1577,7 +1597,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="8" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>6</v>
       </c>
@@ -1600,12 +1620,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="11" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C5" s="13" t="s">
         <v>18</v>
@@ -1621,12 +1641,12 @@
       </c>
       <c r="G5" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>18</v>
@@ -1641,12 +1661,12 @@
         <v>96</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="8" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" s="8" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>18</v>
@@ -1662,30 +1682,30 @@
       </c>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="1:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C8" s="1" t="s">
+    <row r="8" spans="1:7" s="20" customFormat="1" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="C8" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="21">
         <v>44298</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="20" t="s">
         <v>103</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="19" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
@@ -1708,7 +1728,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
@@ -1731,7 +1751,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
@@ -1754,7 +1774,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>9</v>
       </c>
@@ -1775,7 +1795,7 @@
       </c>
       <c r="G12" s="7"/>
     </row>
-    <row r="13" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>10</v>
       </c>
@@ -1795,7 +1815,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>10</v>
       </c>
@@ -1815,7 +1835,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>10</v>
       </c>
@@ -1835,7 +1855,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>10</v>
       </c>
@@ -1855,7 +1875,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>10</v>
       </c>
@@ -1875,7 +1895,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>10</v>
       </c>
@@ -1898,7 +1918,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>10</v>
       </c>
@@ -1921,7 +1941,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>10</v>
       </c>
@@ -1944,7 +1964,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>10</v>
       </c>
@@ -1967,7 +1987,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>10</v>
       </c>
@@ -1990,7 +2010,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>10</v>
       </c>
@@ -2013,7 +2033,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>10</v>
       </c>
@@ -2033,7 +2053,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>10</v>
       </c>
@@ -2056,7 +2076,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>10</v>
       </c>
@@ -2078,7 +2098,7 @@
       <c r="K26" s="4"/>
       <c r="L26" s="4"/>
     </row>
-    <row r="27" spans="1:12" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>10</v>
       </c>
@@ -2104,7 +2124,7 @@
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
     </row>
-    <row r="28" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>10</v>
       </c>
@@ -2124,7 +2144,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>10</v>
       </c>
@@ -2144,7 +2164,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>10</v>
       </c>
@@ -2164,7 +2184,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>10</v>
       </c>
@@ -2187,7 +2207,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>10</v>
       </c>
@@ -2210,7 +2230,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>10</v>
       </c>
@@ -2233,7 +2253,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>10</v>
       </c>
@@ -2256,7 +2276,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>10</v>
       </c>
@@ -2279,7 +2299,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>10</v>
       </c>
@@ -2302,7 +2322,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>10</v>
       </c>
@@ -2325,7 +2345,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>10</v>
       </c>
@@ -2348,7 +2368,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>10</v>
       </c>
@@ -2371,7 +2391,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="40" spans="1:7" s="8" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" s="8" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>10</v>
       </c>
@@ -2394,7 +2414,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>11</v>
       </c>
@@ -2414,7 +2434,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>11</v>
       </c>
@@ -2437,7 +2457,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="43" spans="1:7" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
         <v>11</v>
       </c>
@@ -2458,7 +2478,7 @@
       </c>
       <c r="G43" s="7"/>
     </row>
-    <row r="44" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>15</v>
       </c>
@@ -2478,7 +2498,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>15</v>
       </c>
@@ -2498,12 +2518,12 @@
         <v>93</v>
       </c>
     </row>
-    <row r="46" spans="1:7" s="5" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" s="5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>20</v>
@@ -2521,7 +2541,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="47" spans="1:7" s="5" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>15</v>
       </c>
@@ -2544,7 +2564,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="48" spans="1:7" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>15</v>
       </c>
@@ -2618,92 +2638,92 @@
       <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="16" max="16" width="73.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="73.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="16:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="16:16" x14ac:dyDescent="0.25">
       <c r="P1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="16:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="16:16" x14ac:dyDescent="0.25">
       <c r="P2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="16:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="16:16" x14ac:dyDescent="0.25">
       <c r="P3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="16:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="16:16" x14ac:dyDescent="0.25">
       <c r="P4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="16:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="16:16" x14ac:dyDescent="0.25">
       <c r="P5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="16:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="16:16" x14ac:dyDescent="0.25">
       <c r="P6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="16:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="16:16" x14ac:dyDescent="0.25">
       <c r="P7" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="16:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="16:16" x14ac:dyDescent="0.25">
       <c r="P8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="16:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="16:16" x14ac:dyDescent="0.25">
       <c r="P9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="16:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="16:16" x14ac:dyDescent="0.25">
       <c r="P10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="16:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="16:16" x14ac:dyDescent="0.25">
       <c r="P11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="16:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="16:16" x14ac:dyDescent="0.25">
       <c r="P12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="16:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="16:16" x14ac:dyDescent="0.25">
       <c r="P14" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="16:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="16:16" x14ac:dyDescent="0.25">
       <c r="P15" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="16:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="16:16" x14ac:dyDescent="0.25">
       <c r="P16" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="16:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="16:16" x14ac:dyDescent="0.25">
       <c r="P17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="16:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="16:16" x14ac:dyDescent="0.25">
       <c r="P18" t="s">
         <v>20</v>
       </c>
@@ -2728,9 +2748,9 @@
       <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="17:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="17:17" x14ac:dyDescent="0.25">
       <c r="Q1" t="s">
         <v>21</v>
       </c>

</xml_diff>